<commit_message>
added eval strategy and fixed issue with dot/ + new sample.bpmn
</commit_message>
<xml_diff>
--- a/Notebooks/output.xlsx
+++ b/Notebooks/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,93 +449,151 @@
           <t>Column3</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.5735183104355513</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6459396962749736</v>
+        <v>0.4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3338049409120114</v>
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1301558153317501</v>
+        <v>0.5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5240577975315932</v>
+        <v>0.9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4314101788536073</v>
+        <v>0.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.5640226974662833</v>
+        <v>0.4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.03709113029083788</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5416557578751473</v>
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.7249781866857276</v>
+        <v>0.8</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9967886791562257</v>
+        <v>0.8</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2101229971576437</v>
+        <v>0.3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.02585099569197236</v>
+        <v>0.6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7009003110126709</v>
+        <v>0.8</v>
       </c>
       <c r="C6" t="n">
-        <v>0.008570351949527932</v>
+        <v>0.6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.02850842109081964</v>
+        <v>0.2</v>
       </c>
       <c r="B7" t="n">
-        <v>0.7201425735377773</v>
+        <v>0.5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.07673646195855655</v>
+        <v>0.2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.2350514773064417</v>
+        <v>0.9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1647336708056084</v>
+        <v>0.6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.458076595755007</v>
+        <v>0.3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.0414505635766842</v>
+        <v>0.3</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3914578031432729</v>
+        <v>0.5</v>
       </c>
       <c r="C9" t="n">
-        <v>0.05819178810388181</v>
+        <v>0.6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>